<commit_message>
Product Display Formatting Improvements and other changes
I improved the product display formatting to be aligned and easier to read, for when we create and print an Invoice and show inventory that we looked up. Other useful changes are here as well.
</commit_message>
<xml_diff>
--- a/Product_List.xlsx
+++ b/Product_List.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3bc697bdb8b8b24/Documents/University Documents/CSULB Documents/CSULB CECS Files/CECS 543 Software Engineering/Assignments/Assignment 3/Assignment-3 Github Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4140E3FA-B158-463D-BC5A-351DC22286B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37BA2AE6-50A1-443E-B421-25AE5EC36561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155"/>
   </bookViews>
   <sheets>
-    <sheet name="Product_List_Test_for_Java_CSV" sheetId="1" r:id="rId1"/>
+    <sheet name="Product_List" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Product ID</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Selling Price</t>
-  </si>
-  <si>
-    <t>Cost Price</t>
-  </si>
-  <si>
     <t>Sony TV</t>
   </si>
   <si>
@@ -56,15 +50,39 @@
   </si>
   <si>
     <t>Pioneer Radio</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>SNY110</t>
+  </si>
+  <si>
+    <t>LG220</t>
+  </si>
+  <si>
+    <t>SMSUNG330</t>
+  </si>
+  <si>
+    <t>SNY440</t>
+  </si>
+  <si>
+    <t>BOSSSS556</t>
+  </si>
+  <si>
+    <t>PONEER665</t>
+  </si>
+  <si>
+    <t>Selling Price ($)</t>
+  </si>
+  <si>
+    <t>Cost Price ($)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -544,7 +562,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -900,149 +918,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>900</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>900</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>400</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>100</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>7</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>260</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>3</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>450</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>200</v>
       </c>
     </row>

</xml_diff>